<commit_message>
Update xls files for compatibility wrt changes in code
</commit_message>
<xml_diff>
--- a/misc/FPS_Convection_variables_4_CMOR.xlsx
+++ b/misc/FPS_Convection_variables_4_CMOR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="295">
   <si>
     <t>CCLM variable name</t>
   </si>
@@ -850,18 +850,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Sum over 8 levels from ground to 2.86 m depth</t>
-  </si>
-  <si>
-    <t>depth of first soil layer: 0.5 cm</t>
-  </si>
-  <si>
-    <t>height is above ground</t>
-  </si>
-  <si>
-    <t>ECMWF method used for calculating psl</t>
-  </si>
-  <si>
     <t>CIN_ML</t>
   </si>
   <si>
@@ -893,6 +881,30 @@
   </si>
   <si>
     <t>Additional subdaily frq[1/day]</t>
+  </si>
+  <si>
+    <t>atmosphere_convective_available_potential_energy_wrt_surface</t>
+  </si>
+  <si>
+    <t>ECMWF method used for psl calculation</t>
+  </si>
+  <si>
+    <t>CAPE based on a parcel with thermodynamical properties of a 50hPa deep mixed layer in the PBL</t>
+  </si>
+  <si>
+    <t>CIN based on a parcel with thermodynamical properties of a 50hPa deep mixed layer in the PBL</t>
+  </si>
+  <si>
+    <t>already derotated</t>
+  </si>
+  <si>
+    <t>already derotated; height is above ground</t>
+  </si>
+  <si>
+    <t>depth of first soil layer: 1.0 cm</t>
+  </si>
+  <si>
+    <t>Sum over 8 levels from ground to 3.82 m depth</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1802,7 @@
     <col min="24" max="24" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="59.140625" customWidth="1"/>
     <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="71" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="27.140625" bestFit="1" customWidth="1"/>
@@ -1816,10 +1828,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1840,7 +1852,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -1928,8 +1940,11 @@
       <c r="Y2" t="s">
         <v>266</v>
       </c>
+      <c r="Z2" t="s">
+        <v>289</v>
+      </c>
       <c r="AA2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="AC2" t="s">
         <v>33</v>
@@ -1937,10 +1952,10 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C3" t="s">
         <v>268</v>
@@ -1975,6 +1990,9 @@
       <c r="Y3" t="s">
         <v>269</v>
       </c>
+      <c r="Z3" t="s">
+        <v>290</v>
+      </c>
       <c r="AA3" t="s">
         <v>267</v>
       </c>
@@ -1984,13 +2002,13 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -2023,10 +2041,10 @@
         <v>43</v>
       </c>
       <c r="Y4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="AC4" t="s">
         <v>33</v>
@@ -2343,7 +2361,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
         <v>125</v>
@@ -2794,7 +2812,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -2844,7 +2862,7 @@
         <v>236</v>
       </c>
       <c r="Z20" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="AA20" t="s">
         <v>237</v>
@@ -2903,7 +2921,7 @@
         <v>233</v>
       </c>
       <c r="Z21" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="AA21" t="s">
         <v>234</v>
@@ -3135,7 +3153,7 @@
         <v>172</v>
       </c>
       <c r="Z26" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="AA26" t="s">
         <v>173</v>
@@ -4087,6 +4105,9 @@
       <c r="Y45" t="s">
         <v>74</v>
       </c>
+      <c r="Z45" t="s">
+        <v>291</v>
+      </c>
       <c r="AA45" t="s">
         <v>67</v>
       </c>
@@ -4141,7 +4162,7 @@
         <v>70</v>
       </c>
       <c r="Z46" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="AA46" t="s">
         <v>67</v>
@@ -4196,6 +4217,9 @@
       <c r="Y47" t="s">
         <v>74</v>
       </c>
+      <c r="Z47" t="s">
+        <v>291</v>
+      </c>
       <c r="AA47" t="s">
         <v>67</v>
       </c>
@@ -4249,6 +4273,9 @@
       <c r="Y48" t="s">
         <v>74</v>
       </c>
+      <c r="Z48" t="s">
+        <v>291</v>
+      </c>
       <c r="AA48" t="s">
         <v>67</v>
       </c>
@@ -4302,6 +4329,9 @@
       <c r="Y49" t="s">
         <v>74</v>
       </c>
+      <c r="Z49" t="s">
+        <v>291</v>
+      </c>
       <c r="AA49" t="s">
         <v>67</v>
       </c>
@@ -4355,6 +4385,9 @@
       <c r="Y50" t="s">
         <v>74</v>
       </c>
+      <c r="Z50" t="s">
+        <v>291</v>
+      </c>
       <c r="AA50" t="s">
         <v>67</v>
       </c>
@@ -4408,6 +4441,9 @@
       <c r="Y51" t="s">
         <v>74</v>
       </c>
+      <c r="Z51" t="s">
+        <v>291</v>
+      </c>
       <c r="AA51" t="s">
         <v>67</v>
       </c>
@@ -4461,6 +4497,9 @@
       <c r="Y52" t="s">
         <v>66</v>
       </c>
+      <c r="Z52" t="s">
+        <v>291</v>
+      </c>
       <c r="AA52" t="s">
         <v>67</v>
       </c>
@@ -4514,6 +4553,9 @@
       <c r="Y53" t="s">
         <v>94</v>
       </c>
+      <c r="Z53" t="s">
+        <v>291</v>
+      </c>
       <c r="AA53" t="s">
         <v>88</v>
       </c>
@@ -4568,7 +4610,7 @@
         <v>91</v>
       </c>
       <c r="Z54" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="AA54" t="s">
         <v>88</v>
@@ -4623,6 +4665,9 @@
       <c r="Y55" t="s">
         <v>94</v>
       </c>
+      <c r="Z55" t="s">
+        <v>291</v>
+      </c>
       <c r="AA55" t="s">
         <v>88</v>
       </c>
@@ -4676,6 +4721,9 @@
       <c r="Y56" t="s">
         <v>94</v>
       </c>
+      <c r="Z56" t="s">
+        <v>291</v>
+      </c>
       <c r="AA56" t="s">
         <v>88</v>
       </c>
@@ -4729,6 +4777,9 @@
       <c r="Y57" t="s">
         <v>94</v>
       </c>
+      <c r="Z57" t="s">
+        <v>291</v>
+      </c>
       <c r="AA57" t="s">
         <v>88</v>
       </c>
@@ -4782,6 +4833,9 @@
       <c r="Y58" t="s">
         <v>94</v>
       </c>
+      <c r="Z58" t="s">
+        <v>291</v>
+      </c>
       <c r="AA58" t="s">
         <v>88</v>
       </c>
@@ -4835,6 +4889,9 @@
       <c r="Y59" t="s">
         <v>94</v>
       </c>
+      <c r="Z59" t="s">
+        <v>291</v>
+      </c>
       <c r="AA59" t="s">
         <v>88</v>
       </c>
@@ -4888,6 +4945,9 @@
       <c r="Y60" t="s">
         <v>87</v>
       </c>
+      <c r="Z60" t="s">
+        <v>291</v>
+      </c>
       <c r="AA60" t="s">
         <v>88</v>
       </c>
@@ -5471,13 +5531,13 @@
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B72" t="s">
         <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F72" t="s">
         <v>73</v>

</xml_diff>